<commit_message>
Read user remarks in 6800 Excel files
</commit_message>
<xml_diff>
--- a/inst/extdata/c3_aci_1.xlsx
+++ b/inst/extdata/c3_aci_1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Measurements" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="617">
   <si>
     <t>File opened</t>
   </si>
@@ -1859,6 +1859,18 @@
   </si>
   <si>
     <t>5a</t>
+  </si>
+  <si>
+    <t>11:04:20</t>
+  </si>
+  <si>
+    <t>a user remark</t>
+  </si>
+  <si>
+    <t>13:10:42</t>
+  </si>
+  <si>
+    <t>another user remark</t>
   </si>
 </sst>
 </file>
@@ -1894,8 +1906,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2202,7 +2215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IE64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -41173,9 +41186,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -41291,7 +41306,24 @@
         <v>24</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="B15" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="B16" t="s">
+        <v>616</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>